<commit_message>
working on pairing observations
</commit_message>
<xml_diff>
--- a/data/davis matches/davis_2018.xlsx
+++ b/data/davis matches/davis_2018.xlsx
@@ -10972,21 +10972,9 @@
         </is>
       </c>
       <c r="T117" t="inlineStr"/>
-      <c r="U117" t="inlineStr">
-        <is>
-          <t>USA</t>
-        </is>
-      </c>
-      <c r="V117" t="inlineStr">
-        <is>
-          <t>20 Jan 1998</t>
-        </is>
-      </c>
-      <c r="W117" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
+      <c r="U117" t="inlineStr"/>
+      <c r="V117" t="inlineStr"/>
+      <c r="W117" t="inlineStr"/>
       <c r="X117" t="inlineStr"/>
       <c r="Y117" t="inlineStr"/>
       <c r="Z117" t="inlineStr"/>
@@ -11524,21 +11512,9 @@
         </is>
       </c>
       <c r="T123" t="inlineStr"/>
-      <c r="U123" t="inlineStr">
-        <is>
-          <t>USA</t>
-        </is>
-      </c>
-      <c r="V123" t="inlineStr">
-        <is>
-          <t>20 Jan 1998</t>
-        </is>
-      </c>
-      <c r="W123" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
+      <c r="U123" t="inlineStr"/>
+      <c r="V123" t="inlineStr"/>
+      <c r="W123" t="inlineStr"/>
       <c r="X123" t="inlineStr"/>
       <c r="Y123" t="inlineStr"/>
       <c r="Z123" t="inlineStr"/>

</xml_diff>